<commit_message>
add Circuit schematic & Bills of material
</commit_message>
<xml_diff>
--- a/Circuit_Schematic/Embeded_System.xlsx
+++ b/Circuit_Schematic/Embeded_System.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RanShy\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B8634D-27D7-4EA9-B2A5-C1D0CE7515C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F99092CE-3453-43A5-ACDF-3FDA197E21EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2544" yWindow="0" windowWidth="16308" windowHeight="8280" xr2:uid="{C68507AB-7EA3-4CCA-BF59-5D8B0DCE7847}"/>
+    <workbookView xWindow="1272" yWindow="0" windowWidth="16308" windowHeight="8280" xr2:uid="{4D3760B6-B564-4B38-97E4-0DF39038C122}"/>
   </bookViews>
   <sheets>
     <sheet name="Embeded_System" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>Comment</t>
   </si>
@@ -84,13 +84,19 @@
     <t>ServoMotor</t>
   </si>
   <si>
-    <t>ServoMotor_1, ServoMotor_2</t>
+    <t>ServoMotor_1</t>
   </si>
   <si>
     <t>SR04</t>
   </si>
   <si>
     <t>SR0_1, SR04_2</t>
+  </si>
+  <si>
+    <t>Human_Sensor</t>
+  </si>
+  <si>
+    <t>U</t>
   </si>
   <si>
     <t>PysicalPin</t>
@@ -501,18 +507,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E5443C-18BB-4CCF-9445-8AF2FFF9AE8E}">
-  <dimension ref="A1:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76863FE4-1F05-4947-B474-714E4FD4B924}">
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="41.21875" customWidth="1"/>
-    <col min="4" max="6" width="19" customWidth="1"/>
+    <col min="1" max="6" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -612,7 +614,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -649,7 +651,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
@@ -657,21 +659,41 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="F8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>